<commit_message>
Last Version of the game
</commit_message>
<xml_diff>
--- a/Frogger/Testing report.xlsx
+++ b/Frogger/Testing report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="104">
   <si>
     <t>ITERATIVE DEVELOPMENT STEPS</t>
   </si>
@@ -257,9 +257,6 @@
     <t>TESTING REPORT</t>
   </si>
   <si>
-    <t>Testing Number</t>
-  </si>
-  <si>
     <t>IDS tested</t>
   </si>
   <si>
@@ -291,6 +288,45 @@
   </si>
   <si>
     <t>Method .setDefaultCloseOperation() was set to DO_NOTHING_ON_CLOSE, necessary set it to EXIT_ON_CLOSE</t>
+  </si>
+  <si>
+    <t>Missing applying the method dispose() to the JFrame object</t>
+  </si>
+  <si>
+    <t>Missing add the Graphics object to the game Canvas</t>
+  </si>
+  <si>
+    <t>Missing add the Canvas object to the Frame window</t>
+  </si>
+  <si>
+    <t>Wrong math</t>
+  </si>
+  <si>
+    <t>Missing adding and creating a bufferStartegy to the canvas of the game</t>
+  </si>
+  <si>
+    <t>Missing Graphics g as a parameters for the render class</t>
+  </si>
+  <si>
+    <t>Missing implement the variables to record which key was pressed</t>
+  </si>
+  <si>
+    <t>Wrong assignment to the variables when a key is pressed</t>
+  </si>
+  <si>
+    <t>Using keyTyped() methods instead of keyPressed method()</t>
+  </si>
+  <si>
+    <t>Wrong declaration of the path of the file</t>
+  </si>
+  <si>
+    <t>Wrong declaration of the image coordinates</t>
+  </si>
+  <si>
+    <t>Wrong definition of getState() and setState() methods in the State class</t>
+  </si>
+  <si>
+    <t>Test Number</t>
   </si>
 </sst>
 </file>
@@ -389,12 +425,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -403,6 +433,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -721,10 +757,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
+      <c r="B1" s="7"/>
     </row>
     <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -775,7 +811,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.3">
@@ -784,7 +820,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.3">
@@ -1458,12 +1494,12 @@
   <dimension ref="A1:E152"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B152"/>
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="123.77734375" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
@@ -1471,67 +1507,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>81</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="4">
         <v>1</v>
       </c>
-      <c r="C3" s="8" t="str">
-        <f>IF(ISBLANK(B3),"",VLOOKUP(B3,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
+      <c r="C3" s="6" t="str">
+        <f>IF(B3="","",VLOOKUP(B3,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
         <v>Creating the launcher class using the main method, printing something on the command line from it</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="E3" s="7" t="s">
+      <c r="D3" s="4" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.3">
+      <c r="E3" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <f>A3+1</f>
         <v>2</v>
       </c>
-      <c r="B4" s="6">
-        <f>IF(D3="Check",B3+1,B3)</f>
+      <c r="B4" s="4">
+        <f>IF(ISBLANK(D3),"",IF(D3="Check",B3+1,IF(D3="Fail",B3,"Error")))</f>
         <v>2</v>
       </c>
-      <c r="C4" s="8" t="str">
-        <f>IF(ISBLANK(B4),"",VLOOKUP(B4,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
+      <c r="C4" s="6" t="str">
+        <f>IF(B4="","",IF(B4="Error","-",VLOOKUP(B4,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
         <v>Creating the Game class and its start method, instantiate and start it from the Launcher method, print something on command line from the start method</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="E4" s="7" t="s">
+      <c r="D4" s="4" t="s">
         <v>84</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -1539,19 +1575,19 @@
         <f t="shared" ref="A5:A68" si="0">A4+1</f>
         <v>3</v>
       </c>
-      <c r="B5" s="6">
-        <f t="shared" ref="B5:B68" si="1">IF(D4="Check",B4+1,B4)</f>
+      <c r="B5" s="4">
+        <f t="shared" ref="B5:B68" si="1">IF(ISBLANK(D4),"",IF(D4="Check",B4+1,IF(D4="Fail",B4,"Error")))</f>
         <v>3</v>
       </c>
-      <c r="C5" s="8" t="str">
-        <f>IF(ISBLANK(B5),"",VLOOKUP(B5,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
+      <c r="C5" s="6" t="str">
+        <f>IF(B5="","",IF(B5="Error","-",VLOOKUP(B5,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
         <v>Creating a method inside the Game class that starts a window using a Jframe and Canvas object</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>86</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -1559,59 +1595,59 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="4">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="C6" s="8" t="str">
-        <f>IF(ISBLANK(B6),"",VLOOKUP(B6,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
+      <c r="C6" s="6" t="str">
+        <f>IF(B6="","",IF(B6="Error","-",VLOOKUP(B6,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
         <v>Creating a method inside the Game class that starts a window using a Jframe and Canvas object</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="4">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="C7" s="6" t="str">
+        <f>IF(B7="","",IF(B7="Error","-",VLOOKUP(B7,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v>Creating a Display class that will hold the methods to initiate and close the game window, instantiate it from the game class and starting the window from it</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E7" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="4">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="C8" s="6" t="str">
+        <f>IF(B8="","",IF(B8="Error","-",VLOOKUP(B8,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v>Creating a Display class that will hold the methods to initiate and close the game window, instantiate it from the game class and starting the window from it</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B7" s="6">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="C7" s="8" t="str">
-        <f>IF(ISBLANK(B7),"",VLOOKUP(B7,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Creating a Display class that will hold the methods to initiate and close the game window, instantiate it from the game class and starting the window from it</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B8" s="6">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="C8" s="8" t="str">
-        <f>IF(ISBLANK(B8),"",VLOOKUP(B8,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Creating a Display class that will hold the methods to initiate and close the game window, instantiate it from the game class and starting the window from it</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>84</v>
+      <c r="E8" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -1619,19 +1655,19 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="4">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="C9" s="8" t="str">
-        <f>IF(ISBLANK(B9),"",VLOOKUP(B9,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
+      <c r="C9" s="6" t="str">
+        <f>IF(B9="","",IF(B9="Error","-",VLOOKUP(B9,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
         <v>Implementing a thread in the game and starting it from the thread run() method</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="E9" s="7" t="s">
+      <c r="D9" s="4" t="s">
         <v>84</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -1639,19 +1675,19 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="4">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="C10" s="8" t="str">
-        <f>IF(ISBLANK(B10),"",VLOOKUP(B10,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
+      <c r="C10" s="6" t="str">
+        <f>IF(B10="","",IF(B10="Error","-",VLOOKUP(B10,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
         <v>Creating the scope for the game loop in the run() method</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="E10" s="7" t="s">
+      <c r="D10" s="4" t="s">
         <v>84</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.3">
@@ -1659,19 +1695,19 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="4">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="C11" s="8" t="str">
-        <f>IF(ISBLANK(B11),"",VLOOKUP(B11,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
+      <c r="C11" s="6" t="str">
+        <f>IF(B11="","",IF(B11="Error","-",VLOOKUP(B11,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
         <v>Testing closing the game by the close button</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>91</v>
+      <c r="D11" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -1679,37 +1715,39 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="4">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="C12" s="8" t="str">
-        <f>IF(ISBLANK(B12),"",VLOOKUP(B12,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
+      <c r="C12" s="6" t="str">
+        <f>IF(B12="","",IF(B12="Error","-",VLOOKUP(B12,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
         <v>Testing closing the game by the close button</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B13" s="4">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="C13" s="6" t="str">
+        <f>IF(B13="","",IF(B13="Error","-",VLOOKUP(B13,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v>Testing closing the game using a simple timer and stoping the thread</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E12" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B13" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C13" s="8" t="str">
-        <f>IF(ISBLANK(B13),"",VLOOKUP(B13,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="7" t="s">
-        <v>84</v>
+      <c r="E13" s="5" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -1717,17 +1755,19 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="4">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="C14" s="8" t="str">
-        <f>IF(ISBLANK(B14),"",VLOOKUP(B14,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
+      <c r="C14" s="6" t="str">
+        <f>IF(B14="","",IF(B14="Error","-",VLOOKUP(B14,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
         <v>Testing closing the game using a simple timer and stoping the thread</v>
       </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="7" t="s">
+      <c r="D14" s="4" t="s">
         <v>84</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -1735,53 +1775,59 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B15" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C15" s="8" t="str">
-        <f>IF(ISBLANK(B15),"",VLOOKUP(B15,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="7" t="s">
+      <c r="B15" s="4">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="C15" s="6" t="str">
+        <f>IF(B15="","",IF(B15="Error","-",VLOOKUP(B15,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v>Creating a stop method in the game class and using it to close the game</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="E15" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B16" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C16" s="8" t="str">
-        <f>IF(ISBLANK(B16),"",VLOOKUP(B16,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="B16" s="4">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="C16" s="6" t="str">
+        <f>IF(B16="","",IF(B16="Error","-",VLOOKUP(B16,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v>Draw a simple rectangle on the screen</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B17" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C17" s="8" t="str">
-        <f>IF(ISBLANK(B17),"",VLOOKUP(B17,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="7" t="s">
-        <v>84</v>
+      <c r="B17" s="4">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="C17" s="6" t="str">
+        <f>IF(B17="","",IF(B17="Error","-",VLOOKUP(B17,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v>Draw a simple rectangle on the screen</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -1789,17 +1835,19 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B18" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C18" s="8" t="str">
-        <f>IF(ISBLANK(B18),"",VLOOKUP(B18,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="7" t="s">
+      <c r="B18" s="4">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="C18" s="6" t="str">
+        <f>IF(B18="","",IF(B18="Error","-",VLOOKUP(B18,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v>Draw a simple rectangle on the screen</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>84</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -1807,17 +1855,19 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B19" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C19" s="8" t="str">
-        <f>IF(ISBLANK(B19),"",VLOOKUP(B19,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="7" t="s">
-        <v>84</v>
+      <c r="B19" s="4">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="C19" s="6" t="str">
+        <f>IF(B19="","",IF(B19="Error","-",VLOOKUP(B19,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v>Configuring the game loop to run at 60 frames per second</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -1825,17 +1875,19 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B20" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C20" s="8" t="str">
-        <f>IF(ISBLANK(B20),"",VLOOKUP(B20,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D20" s="6"/>
-      <c r="E20" s="7" t="s">
+      <c r="B20" s="4">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="C20" s="6" t="str">
+        <f>IF(B20="","",IF(B20="Error","-",VLOOKUP(B20,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v>Configuring the game loop to run at 60 frames per second</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>84</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -1843,53 +1895,59 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B21" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C21" s="8" t="str">
-        <f>IF(ISBLANK(B21),"",VLOOKUP(B21,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="7" t="s">
+      <c r="B21" s="4">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="C21" s="6" t="str">
+        <f>IF(B21="","",IF(B21="Error","-",VLOOKUP(B21,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v>Creating the tick and render methods in the game class</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="E21" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B22" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C22" s="8" t="str">
-        <f>IF(ISBLANK(B22),"",VLOOKUP(B22,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D22" s="6"/>
-      <c r="E22" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="B22" s="4">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="C22" s="6" t="str">
+        <f>IF(B22="","",IF(B22="Error","-",VLOOKUP(B22,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v>Implementing a bufferedStrategy to draw images on the screen, draw the images through the render method</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B23" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C23" s="8" t="str">
-        <f>IF(ISBLANK(B23),"",VLOOKUP(B23,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D23" s="6"/>
-      <c r="E23" s="7" t="s">
-        <v>84</v>
+      <c r="B23" s="4">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="C23" s="6" t="str">
+        <f>IF(B23="","",IF(B23="Error","-",VLOOKUP(B23,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v>Implementing a bufferedStrategy to draw images on the screen, draw the images through the render method</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -1897,71 +1955,79 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B24" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C24" s="8" t="str">
-        <f>IF(ISBLANK(B24),"",VLOOKUP(B24,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="7" t="s">
+      <c r="B24" s="4">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="C24" s="6" t="str">
+        <f>IF(B24="","",IF(B24="Error","-",VLOOKUP(B24,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v>Implementing a bufferedStrategy to draw images on the screen, draw the images through the render method</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="E24" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B25" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C25" s="8" t="str">
-        <f>IF(ISBLANK(B25),"",VLOOKUP(B25,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D25" s="6"/>
-      <c r="E25" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="B25" s="4">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="C25" s="6" t="str">
+        <f>IF(B25="","",IF(B25="Error","-",VLOOKUP(B25,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v>Creating the KeyListener class, instatiating it on the game class and using it to print objects on the screen</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B26" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C26" s="8" t="str">
-        <f>IF(ISBLANK(B26),"",VLOOKUP(B26,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D26" s="6"/>
-      <c r="E26" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="B26" s="4">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="C26" s="6" t="str">
+        <f>IF(B26="","",IF(B26="Error","-",VLOOKUP(B26,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v>Creating the KeyListener class, instatiating it on the game class and using it to print objects on the screen</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B27" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C27" s="8" t="str">
-        <f>IF(ISBLANK(B27),"",VLOOKUP(B27,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D27" s="6"/>
-      <c r="E27" s="7" t="s">
-        <v>84</v>
+      <c r="B27" s="4">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="C27" s="6" t="str">
+        <f>IF(B27="","",IF(B27="Error","-",VLOOKUP(B27,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v>Creating the KeyListener class, instatiating it on the game class and using it to print objects on the screen</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -1969,17 +2035,19 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B28" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C28" s="8" t="str">
-        <f>IF(ISBLANK(B28),"",VLOOKUP(B28,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D28" s="6"/>
-      <c r="E28" s="7" t="s">
+      <c r="B28" s="4">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="C28" s="6" t="str">
+        <f>IF(B28="","",IF(B28="Error","-",VLOOKUP(B28,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v>Creating the KeyListener class, instatiating it on the game class and using it to print objects on the screen</v>
+      </c>
+      <c r="D28" s="4" t="s">
         <v>84</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -1987,89 +2055,99 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B29" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C29" s="8" t="str">
-        <f>IF(ISBLANK(B29),"",VLOOKUP(B29,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D29" s="6"/>
-      <c r="E29" s="7" t="s">
+      <c r="B29" s="4">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="C29" s="6" t="str">
+        <f>IF(B29="","",IF(B29="Error","-",VLOOKUP(B29,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v>Creating the MouseListener class, instatiating it on the game class and using it to printt objects on the screen</v>
+      </c>
+      <c r="D29" s="4" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="E29" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B30" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C30" s="8" t="str">
-        <f>IF(ISBLANK(B30),"",VLOOKUP(B30,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D30" s="6"/>
-      <c r="E30" s="7" t="s">
+      <c r="B30" s="4">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="C30" s="6" t="str">
+        <f>IF(B30="","",IF(B30="Error","-",VLOOKUP(B30,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v>Drawing the images through the render method and making them move on the screen upgranding the position through the tick method</v>
+      </c>
+      <c r="D30" s="4" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="E30" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="B31" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C31" s="8" t="str">
-        <f>IF(ISBLANK(B31),"",VLOOKUP(B31,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D31" s="6"/>
-      <c r="E31" s="7" t="s">
+      <c r="B31" s="4">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="C31" s="6" t="str">
+        <f>IF(B31="","",IF(B31="Error","-",VLOOKUP(B31,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v>Creating a folder that will hold all the sprites of the game, configuring it as a library path</v>
+      </c>
+      <c r="D31" s="4" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="E31" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="B32" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C32" s="8" t="str">
-        <f>IF(ISBLANK(B32),"",VLOOKUP(B32,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D32" s="6"/>
-      <c r="E32" s="7" t="s">
+      <c r="B32" s="4">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="C32" s="6" t="str">
+        <f>IF(B32="","",IF(B32="Error","-",VLOOKUP(B32,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v>Creating the ImageLoader class, loading the entire images and printing them on the screen through the game class render method</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B33" s="4">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="C33" s="6" t="str">
+        <f>IF(B33="","",IF(B33="Error","-",VLOOKUP(B33,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v>Creating the ImageLoader class, loading the entire images and printing them on the screen through the game class render method</v>
+      </c>
+      <c r="D33" s="4" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" ht="15" x14ac:dyDescent="0.3">
-      <c r="A33" s="1">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="B33" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C33" s="8" t="str">
-        <f>IF(ISBLANK(B33),"",VLOOKUP(B33,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D33" s="6"/>
-      <c r="E33" s="7" t="s">
-        <v>84</v>
+      <c r="E33" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2077,53 +2155,59 @@
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="B34" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C34" s="8" t="str">
-        <f>IF(ISBLANK(B34),"",VLOOKUP(B34,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D34" s="6"/>
-      <c r="E34" s="7" t="s">
+      <c r="B34" s="4">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="C34" s="6" t="str">
+        <f>IF(B34="","",IF(B34="Error","-",VLOOKUP(B34,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v>Implementing an SpriteSheet class that will hold the methods to crop the spritesheet in the program</v>
+      </c>
+      <c r="D34" s="4" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="E34" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="B35" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C35" s="8" t="str">
-        <f>IF(ISBLANK(B35),"",VLOOKUP(B35,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D35" s="6"/>
-      <c r="E35" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="B35" s="4">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="C35" s="6" t="str">
+        <f>IF(B35="","",IF(B35="Error","-",VLOOKUP(B35,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v>Creating the Assets class with an init() method that will hold and initiate all the images on the game, calling it from the game class</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="B36" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C36" s="8" t="str">
-        <f>IF(ISBLANK(B36),"",VLOOKUP(B36,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D36" s="6"/>
-      <c r="E36" s="7" t="s">
-        <v>84</v>
+      <c r="B36" s="4">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="C36" s="6" t="str">
+        <f>IF(B36="","",IF(B36="Error","-",VLOOKUP(B36,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v>Creating the Assets class with an init() method that will hold and initiate all the images on the game, calling it from the game class</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2131,17 +2215,19 @@
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="B37" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C37" s="8" t="str">
-        <f>IF(ISBLANK(B37),"",VLOOKUP(B37,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D37" s="6"/>
-      <c r="E37" s="7" t="s">
+      <c r="B37" s="4">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="C37" s="6" t="str">
+        <f>IF(B37="","",IF(B37="Error","-",VLOOKUP(B37,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v>Creating the Assets class with an init() method that will hold and initiate all the images on the game, calling it from the game class</v>
+      </c>
+      <c r="D37" s="4" t="s">
         <v>84</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2149,17 +2235,19 @@
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="B38" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C38" s="8" t="str">
-        <f>IF(ISBLANK(B38),"",VLOOKUP(B38,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D38" s="6"/>
-      <c r="E38" s="7" t="s">
+      <c r="B38" s="4">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="C38" s="6" t="str">
+        <f>IF(B38="","",IF(B38="Error","-",VLOOKUP(B38,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v>Using the Assets class to prin several image on the screen through the game class render method</v>
+      </c>
+      <c r="D38" s="4" t="s">
         <v>84</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2167,17 +2255,19 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="B39" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C39" s="8" t="str">
-        <f>IF(ISBLANK(B39),"",VLOOKUP(B39,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D39" s="6"/>
-      <c r="E39" s="7" t="s">
+      <c r="B39" s="4">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="C39" s="6" t="str">
+        <f>IF(B39="","",IF(B39="Error","-",VLOOKUP(B39,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v>Create an abstract State class with the methods to work with them, using this methods to draw images on the screen</v>
+      </c>
+      <c r="D39" s="4" t="s">
         <v>84</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2185,35 +2275,39 @@
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="B40" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C40" s="8" t="str">
-        <f>IF(ISBLANK(B40),"",VLOOKUP(B40,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D40" s="6"/>
-      <c r="E40" s="7" t="s">
+      <c r="B40" s="4">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="C40" s="6" t="str">
+        <f>IF(B40="","",IF(B40="Error","-",VLOOKUP(B40,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v>Create a GameState class the extends the State class, instantiate it in the game class and defining it as the initial game state</v>
+      </c>
+      <c r="D40" s="4" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" ht="15" x14ac:dyDescent="0.3">
+      <c r="E40" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="B41" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C41" s="8" t="str">
-        <f>IF(ISBLANK(B41),"",VLOOKUP(B41,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D41" s="6"/>
-      <c r="E41" s="7" t="s">
-        <v>84</v>
+      <c r="B41" s="4">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="C41" s="6" t="str">
+        <f>IF(B41="","",IF(B41="Error","-",VLOOKUP(B41,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v>Making the tick and render methods in the game class call the tick and render method defined on the states objects</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2221,17 +2315,19 @@
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="B42" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C42" s="8" t="str">
-        <f>IF(ISBLANK(B42),"",VLOOKUP(B42,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D42" s="6"/>
-      <c r="E42" s="7" t="s">
+      <c r="B42" s="4">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="C42" s="6" t="str">
+        <f>IF(B42="","",IF(B42="Error","-",VLOOKUP(B42,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v>Making the tick and render methods in the game class call the tick and render method defined on the states objects</v>
+      </c>
+      <c r="D42" s="4" t="s">
         <v>84</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2239,17 +2335,19 @@
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="B43" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C43" s="8" t="str">
-        <f>IF(ISBLANK(B43),"",VLOOKUP(B43,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D43" s="6"/>
-      <c r="E43" s="7" t="s">
+      <c r="B43" s="4">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="C43" s="6" t="str">
+        <f>IF(B43="","",IF(B43="Error","-",VLOOKUP(B43,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v>Drawing an image on the screen and making it move using the GameState class tick and render methods</v>
+      </c>
+      <c r="D43" s="4" t="s">
         <v>84</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2257,17 +2355,17 @@
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="B44" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C44" s="8" t="str">
-        <f>IF(ISBLANK(B44),"",VLOOKUP(B44,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D44" s="6"/>
-      <c r="E44" s="7" t="s">
-        <v>84</v>
+      <c r="B44" s="4">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="C44" s="6" t="str">
+        <f>IF(B44="","",IF(B44="Error","-",VLOOKUP(B44,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v>Creating the Entity class the will hold all the common information for the entities in the game</v>
+      </c>
+      <c r="D44" s="4"/>
+      <c r="E44" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2275,17 +2373,17 @@
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="B45" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C45" s="8" t="str">
-        <f>IF(ISBLANK(B45),"",VLOOKUP(B45,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D45" s="6"/>
-      <c r="E45" s="7" t="s">
-        <v>84</v>
+      <c r="B45" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C45" s="6" t="str">
+        <f>IF(B45="","",IF(B45="Error","-",VLOOKUP(B45,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D45" s="4"/>
+      <c r="E45" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2293,17 +2391,17 @@
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="B46" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C46" s="8" t="str">
-        <f>IF(ISBLANK(B46),"",VLOOKUP(B46,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D46" s="6"/>
-      <c r="E46" s="7" t="s">
-        <v>84</v>
+      <c r="B46" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C46" s="6" t="str">
+        <f>IF(B46="","",IF(B46="Error","-",VLOOKUP(B46,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D46" s="4"/>
+      <c r="E46" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2311,17 +2409,17 @@
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="B47" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C47" s="8" t="str">
-        <f>IF(ISBLANK(B47),"",VLOOKUP(B47,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D47" s="6"/>
-      <c r="E47" s="7" t="s">
-        <v>84</v>
+      <c r="B47" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C47" s="6" t="str">
+        <f>IF(B47="","",IF(B47="Error","-",VLOOKUP(B47,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D47" s="4"/>
+      <c r="E47" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2329,17 +2427,17 @@
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="B48" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C48" s="8" t="str">
-        <f>IF(ISBLANK(B48),"",VLOOKUP(B48,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D48" s="6"/>
-      <c r="E48" s="7" t="s">
-        <v>84</v>
+      <c r="B48" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C48" s="6" t="str">
+        <f>IF(B48="","",IF(B48="Error","-",VLOOKUP(B48,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D48" s="4"/>
+      <c r="E48" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2347,17 +2445,17 @@
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="B49" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C49" s="8" t="str">
-        <f>IF(ISBLANK(B49),"",VLOOKUP(B49,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D49" s="6"/>
-      <c r="E49" s="7" t="s">
-        <v>84</v>
+      <c r="B49" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C49" s="6" t="str">
+        <f>IF(B49="","",IF(B49="Error","-",VLOOKUP(B49,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D49" s="4"/>
+      <c r="E49" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2365,17 +2463,17 @@
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="B50" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C50" s="8" t="str">
-        <f>IF(ISBLANK(B50),"",VLOOKUP(B50,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D50" s="6"/>
-      <c r="E50" s="7" t="s">
-        <v>84</v>
+      <c r="B50" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C50" s="6" t="str">
+        <f>IF(B50="","",IF(B50="Error","-",VLOOKUP(B50,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D50" s="4"/>
+      <c r="E50" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2383,17 +2481,17 @@
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="B51" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C51" s="8" t="str">
-        <f>IF(ISBLANK(B51),"",VLOOKUP(B51,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D51" s="6"/>
-      <c r="E51" s="7" t="s">
-        <v>84</v>
+      <c r="B51" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C51" s="6" t="str">
+        <f>IF(B51="","",IF(B51="Error","-",VLOOKUP(B51,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D51" s="4"/>
+      <c r="E51" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2401,17 +2499,17 @@
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="B52" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C52" s="8" t="str">
-        <f>IF(ISBLANK(B52),"",VLOOKUP(B52,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D52" s="6"/>
-      <c r="E52" s="7" t="s">
-        <v>84</v>
+      <c r="B52" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C52" s="6" t="str">
+        <f>IF(B52="","",IF(B52="Error","-",VLOOKUP(B52,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D52" s="4"/>
+      <c r="E52" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2419,17 +2517,17 @@
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-      <c r="B53" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C53" s="8" t="str">
-        <f>IF(ISBLANK(B53),"",VLOOKUP(B53,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D53" s="6"/>
-      <c r="E53" s="7" t="s">
-        <v>84</v>
+      <c r="B53" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C53" s="6" t="str">
+        <f>IF(B53="","",IF(B53="Error","-",VLOOKUP(B53,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D53" s="4"/>
+      <c r="E53" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2437,17 +2535,17 @@
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="B54" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C54" s="8" t="str">
-        <f>IF(ISBLANK(B54),"",VLOOKUP(B54,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D54" s="6"/>
-      <c r="E54" s="7" t="s">
-        <v>84</v>
+      <c r="B54" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C54" s="6" t="str">
+        <f>IF(B54="","",IF(B54="Error","-",VLOOKUP(B54,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D54" s="4"/>
+      <c r="E54" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2455,17 +2553,17 @@
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="B55" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C55" s="8" t="str">
-        <f>IF(ISBLANK(B55),"",VLOOKUP(B55,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D55" s="6"/>
-      <c r="E55" s="7" t="s">
-        <v>84</v>
+      <c r="B55" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C55" s="6" t="str">
+        <f>IF(B55="","",IF(B55="Error","-",VLOOKUP(B55,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D55" s="4"/>
+      <c r="E55" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2473,17 +2571,17 @@
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="B56" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C56" s="8" t="str">
-        <f>IF(ISBLANK(B56),"",VLOOKUP(B56,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D56" s="6"/>
-      <c r="E56" s="7" t="s">
-        <v>84</v>
+      <c r="B56" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C56" s="6" t="str">
+        <f>IF(B56="","",IF(B56="Error","-",VLOOKUP(B56,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D56" s="4"/>
+      <c r="E56" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2491,17 +2589,17 @@
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="B57" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C57" s="8" t="str">
-        <f>IF(ISBLANK(B57),"",VLOOKUP(B57,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D57" s="6"/>
-      <c r="E57" s="7" t="s">
-        <v>84</v>
+      <c r="B57" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C57" s="6" t="str">
+        <f>IF(B57="","",IF(B57="Error","-",VLOOKUP(B57,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D57" s="4"/>
+      <c r="E57" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2509,17 +2607,17 @@
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-      <c r="B58" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C58" s="8" t="str">
-        <f>IF(ISBLANK(B58),"",VLOOKUP(B58,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D58" s="6"/>
-      <c r="E58" s="7" t="s">
-        <v>84</v>
+      <c r="B58" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C58" s="6" t="str">
+        <f>IF(B58="","",IF(B58="Error","-",VLOOKUP(B58,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D58" s="4"/>
+      <c r="E58" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2527,17 +2625,17 @@
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
-      <c r="B59" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C59" s="8" t="str">
-        <f>IF(ISBLANK(B59),"",VLOOKUP(B59,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D59" s="6"/>
-      <c r="E59" s="7" t="s">
-        <v>84</v>
+      <c r="B59" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C59" s="6" t="str">
+        <f>IF(B59="","",IF(B59="Error","-",VLOOKUP(B59,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D59" s="4"/>
+      <c r="E59" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2545,17 +2643,17 @@
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
-      <c r="B60" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C60" s="8" t="str">
-        <f>IF(ISBLANK(B60),"",VLOOKUP(B60,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D60" s="6"/>
-      <c r="E60" s="7" t="s">
-        <v>84</v>
+      <c r="B60" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C60" s="6" t="str">
+        <f>IF(B60="","",IF(B60="Error","-",VLOOKUP(B60,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D60" s="4"/>
+      <c r="E60" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2563,17 +2661,17 @@
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
-      <c r="B61" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C61" s="8" t="str">
-        <f>IF(ISBLANK(B61),"",VLOOKUP(B61,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D61" s="6"/>
-      <c r="E61" s="7" t="s">
-        <v>84</v>
+      <c r="B61" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C61" s="6" t="str">
+        <f>IF(B61="","",IF(B61="Error","-",VLOOKUP(B61,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D61" s="4"/>
+      <c r="E61" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2581,17 +2679,17 @@
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="B62" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C62" s="8" t="str">
-        <f>IF(ISBLANK(B62),"",VLOOKUP(B62,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D62" s="6"/>
-      <c r="E62" s="7" t="s">
-        <v>84</v>
+      <c r="B62" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C62" s="6" t="str">
+        <f>IF(B62="","",IF(B62="Error","-",VLOOKUP(B62,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D62" s="4"/>
+      <c r="E62" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2599,17 +2697,17 @@
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="B63" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C63" s="8" t="str">
-        <f>IF(ISBLANK(B63),"",VLOOKUP(B63,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D63" s="6"/>
-      <c r="E63" s="7" t="s">
-        <v>84</v>
+      <c r="B63" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C63" s="6" t="str">
+        <f>IF(B63="","",IF(B63="Error","-",VLOOKUP(B63,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D63" s="4"/>
+      <c r="E63" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2617,17 +2715,17 @@
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
-      <c r="B64" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C64" s="8" t="str">
-        <f>IF(ISBLANK(B64),"",VLOOKUP(B64,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D64" s="6"/>
-      <c r="E64" s="7" t="s">
-        <v>84</v>
+      <c r="B64" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C64" s="6" t="str">
+        <f>IF(B64="","",IF(B64="Error","-",VLOOKUP(B64,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D64" s="4"/>
+      <c r="E64" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2635,17 +2733,17 @@
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="B65" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C65" s="8" t="str">
-        <f>IF(ISBLANK(B65),"",VLOOKUP(B65,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D65" s="6"/>
-      <c r="E65" s="7" t="s">
-        <v>84</v>
+      <c r="B65" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C65" s="6" t="str">
+        <f>IF(B65="","",IF(B65="Error","-",VLOOKUP(B65,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D65" s="4"/>
+      <c r="E65" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2653,17 +2751,17 @@
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-      <c r="B66" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C66" s="8" t="str">
-        <f>IF(ISBLANK(B66),"",VLOOKUP(B66,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D66" s="6"/>
-      <c r="E66" s="7" t="s">
-        <v>84</v>
+      <c r="B66" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C66" s="6" t="str">
+        <f>IF(B66="","",IF(B66="Error","-",VLOOKUP(B66,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D66" s="4"/>
+      <c r="E66" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2671,17 +2769,17 @@
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
-      <c r="B67" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C67" s="8" t="str">
-        <f>IF(ISBLANK(B67),"",VLOOKUP(B67,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D67" s="6"/>
-      <c r="E67" s="7" t="s">
-        <v>84</v>
+      <c r="B67" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C67" s="6" t="str">
+        <f>IF(B67="","",IF(B67="Error","-",VLOOKUP(B67,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D67" s="4"/>
+      <c r="E67" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2689,17 +2787,17 @@
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
-      <c r="B68" s="6">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="C68" s="8" t="str">
-        <f>IF(ISBLANK(B68),"",VLOOKUP(B68,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D68" s="6"/>
-      <c r="E68" s="7" t="s">
-        <v>84</v>
+      <c r="B68" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="C68" s="6" t="str">
+        <f>IF(B68="","",IF(B68="Error","-",VLOOKUP(B68,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D68" s="4"/>
+      <c r="E68" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2707,17 +2805,17 @@
         <f t="shared" ref="A69:A132" si="2">A68+1</f>
         <v>67</v>
       </c>
-      <c r="B69" s="6">
-        <f t="shared" ref="B69:B132" si="3">IF(D68="Check",B68+1,B68)</f>
-        <v>8</v>
-      </c>
-      <c r="C69" s="8" t="str">
-        <f>IF(ISBLANK(B69),"",VLOOKUP(B69,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D69" s="6"/>
-      <c r="E69" s="7" t="s">
-        <v>84</v>
+      <c r="B69" s="4" t="str">
+        <f t="shared" ref="B69:B132" si="3">IF(ISBLANK(D68),"",IF(D68="Check",B68+1,IF(D68="Fail",B68,"Error")))</f>
+        <v/>
+      </c>
+      <c r="C69" s="6" t="str">
+        <f>IF(B69="","",IF(B69="Error","-",VLOOKUP(B69,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D69" s="4"/>
+      <c r="E69" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2725,17 +2823,17 @@
         <f t="shared" si="2"/>
         <v>68</v>
       </c>
-      <c r="B70" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C70" s="8" t="str">
-        <f>IF(ISBLANK(B70),"",VLOOKUP(B70,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D70" s="6"/>
-      <c r="E70" s="7" t="s">
-        <v>84</v>
+      <c r="B70" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C70" s="6" t="str">
+        <f>IF(B70="","",IF(B70="Error","-",VLOOKUP(B70,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D70" s="4"/>
+      <c r="E70" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2743,17 +2841,17 @@
         <f t="shared" si="2"/>
         <v>69</v>
       </c>
-      <c r="B71" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C71" s="8" t="str">
-        <f>IF(ISBLANK(B71),"",VLOOKUP(B71,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D71" s="6"/>
-      <c r="E71" s="7" t="s">
-        <v>84</v>
+      <c r="B71" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C71" s="6" t="str">
+        <f>IF(B71="","",IF(B71="Error","-",VLOOKUP(B71,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D71" s="4"/>
+      <c r="E71" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2761,17 +2859,17 @@
         <f t="shared" si="2"/>
         <v>70</v>
       </c>
-      <c r="B72" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C72" s="8" t="str">
-        <f>IF(ISBLANK(B72),"",VLOOKUP(B72,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D72" s="6"/>
-      <c r="E72" s="7" t="s">
-        <v>84</v>
+      <c r="B72" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C72" s="6" t="str">
+        <f>IF(B72="","",IF(B72="Error","-",VLOOKUP(B72,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D72" s="4"/>
+      <c r="E72" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2779,17 +2877,17 @@
         <f t="shared" si="2"/>
         <v>71</v>
       </c>
-      <c r="B73" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C73" s="8" t="str">
-        <f>IF(ISBLANK(B73),"",VLOOKUP(B73,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D73" s="6"/>
-      <c r="E73" s="7" t="s">
-        <v>84</v>
+      <c r="B73" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C73" s="6" t="str">
+        <f>IF(B73="","",IF(B73="Error","-",VLOOKUP(B73,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D73" s="4"/>
+      <c r="E73" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2797,17 +2895,17 @@
         <f t="shared" si="2"/>
         <v>72</v>
       </c>
-      <c r="B74" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C74" s="8" t="str">
-        <f>IF(ISBLANK(B74),"",VLOOKUP(B74,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D74" s="6"/>
-      <c r="E74" s="7" t="s">
-        <v>84</v>
+      <c r="B74" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C74" s="6" t="str">
+        <f>IF(B74="","",IF(B74="Error","-",VLOOKUP(B74,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D74" s="4"/>
+      <c r="E74" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2815,17 +2913,17 @@
         <f t="shared" si="2"/>
         <v>73</v>
       </c>
-      <c r="B75" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C75" s="8" t="str">
-        <f>IF(ISBLANK(B75),"",VLOOKUP(B75,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D75" s="6"/>
-      <c r="E75" s="7" t="s">
-        <v>84</v>
+      <c r="B75" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C75" s="6" t="str">
+        <f>IF(B75="","",IF(B75="Error","-",VLOOKUP(B75,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D75" s="4"/>
+      <c r="E75" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2833,17 +2931,17 @@
         <f t="shared" si="2"/>
         <v>74</v>
       </c>
-      <c r="B76" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C76" s="8" t="str">
-        <f>IF(ISBLANK(B76),"",VLOOKUP(B76,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D76" s="6"/>
-      <c r="E76" s="7" t="s">
-        <v>84</v>
+      <c r="B76" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C76" s="6" t="str">
+        <f>IF(B76="","",IF(B76="Error","-",VLOOKUP(B76,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D76" s="4"/>
+      <c r="E76" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2851,17 +2949,17 @@
         <f t="shared" si="2"/>
         <v>75</v>
       </c>
-      <c r="B77" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C77" s="8" t="str">
-        <f>IF(ISBLANK(B77),"",VLOOKUP(B77,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D77" s="6"/>
-      <c r="E77" s="7" t="s">
-        <v>84</v>
+      <c r="B77" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C77" s="6" t="str">
+        <f>IF(B77="","",IF(B77="Error","-",VLOOKUP(B77,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D77" s="4"/>
+      <c r="E77" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2869,17 +2967,17 @@
         <f t="shared" si="2"/>
         <v>76</v>
       </c>
-      <c r="B78" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C78" s="8" t="str">
-        <f>IF(ISBLANK(B78),"",VLOOKUP(B78,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D78" s="6"/>
-      <c r="E78" s="7" t="s">
-        <v>84</v>
+      <c r="B78" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C78" s="6" t="str">
+        <f>IF(B78="","",IF(B78="Error","-",VLOOKUP(B78,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D78" s="4"/>
+      <c r="E78" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2887,17 +2985,17 @@
         <f t="shared" si="2"/>
         <v>77</v>
       </c>
-      <c r="B79" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C79" s="8" t="str">
-        <f>IF(ISBLANK(B79),"",VLOOKUP(B79,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D79" s="6"/>
-      <c r="E79" s="7" t="s">
-        <v>84</v>
+      <c r="B79" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C79" s="6" t="str">
+        <f>IF(B79="","",IF(B79="Error","-",VLOOKUP(B79,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D79" s="4"/>
+      <c r="E79" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2905,17 +3003,17 @@
         <f t="shared" si="2"/>
         <v>78</v>
       </c>
-      <c r="B80" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C80" s="8" t="str">
-        <f>IF(ISBLANK(B80),"",VLOOKUP(B80,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D80" s="6"/>
-      <c r="E80" s="7" t="s">
-        <v>84</v>
+      <c r="B80" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C80" s="6" t="str">
+        <f>IF(B80="","",IF(B80="Error","-",VLOOKUP(B80,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D80" s="4"/>
+      <c r="E80" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2923,17 +3021,17 @@
         <f t="shared" si="2"/>
         <v>79</v>
       </c>
-      <c r="B81" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C81" s="8" t="str">
-        <f>IF(ISBLANK(B81),"",VLOOKUP(B81,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D81" s="6"/>
-      <c r="E81" s="7" t="s">
-        <v>84</v>
+      <c r="B81" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C81" s="6" t="str">
+        <f>IF(B81="","",IF(B81="Error","-",VLOOKUP(B81,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D81" s="4"/>
+      <c r="E81" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2941,17 +3039,17 @@
         <f t="shared" si="2"/>
         <v>80</v>
       </c>
-      <c r="B82" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C82" s="8" t="str">
-        <f>IF(ISBLANK(B82),"",VLOOKUP(B82,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D82" s="6"/>
-      <c r="E82" s="7" t="s">
-        <v>84</v>
+      <c r="B82" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C82" s="6" t="str">
+        <f>IF(B82="","",IF(B82="Error","-",VLOOKUP(B82,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D82" s="4"/>
+      <c r="E82" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2959,17 +3057,17 @@
         <f t="shared" si="2"/>
         <v>81</v>
       </c>
-      <c r="B83" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C83" s="8" t="str">
-        <f>IF(ISBLANK(B83),"",VLOOKUP(B83,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D83" s="6"/>
-      <c r="E83" s="7" t="s">
-        <v>84</v>
+      <c r="B83" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C83" s="6" t="str">
+        <f>IF(B83="","",IF(B83="Error","-",VLOOKUP(B83,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D83" s="4"/>
+      <c r="E83" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2977,17 +3075,17 @@
         <f t="shared" si="2"/>
         <v>82</v>
       </c>
-      <c r="B84" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C84" s="8" t="str">
-        <f>IF(ISBLANK(B84),"",VLOOKUP(B84,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D84" s="6"/>
-      <c r="E84" s="7" t="s">
-        <v>84</v>
+      <c r="B84" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C84" s="6" t="str">
+        <f>IF(B84="","",IF(B84="Error","-",VLOOKUP(B84,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D84" s="4"/>
+      <c r="E84" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -2995,17 +3093,17 @@
         <f t="shared" si="2"/>
         <v>83</v>
       </c>
-      <c r="B85" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C85" s="8" t="str">
-        <f>IF(ISBLANK(B85),"",VLOOKUP(B85,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D85" s="6"/>
-      <c r="E85" s="7" t="s">
-        <v>84</v>
+      <c r="B85" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C85" s="6" t="str">
+        <f>IF(B85="","",IF(B85="Error","-",VLOOKUP(B85,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D85" s="4"/>
+      <c r="E85" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3013,17 +3111,17 @@
         <f t="shared" si="2"/>
         <v>84</v>
       </c>
-      <c r="B86" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C86" s="8" t="str">
-        <f>IF(ISBLANK(B86),"",VLOOKUP(B86,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D86" s="6"/>
-      <c r="E86" s="7" t="s">
-        <v>84</v>
+      <c r="B86" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C86" s="6" t="str">
+        <f>IF(B86="","",IF(B86="Error","-",VLOOKUP(B86,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D86" s="4"/>
+      <c r="E86" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3031,17 +3129,17 @@
         <f t="shared" si="2"/>
         <v>85</v>
       </c>
-      <c r="B87" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C87" s="8" t="str">
-        <f>IF(ISBLANK(B87),"",VLOOKUP(B87,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D87" s="6"/>
-      <c r="E87" s="7" t="s">
-        <v>84</v>
+      <c r="B87" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C87" s="6" t="str">
+        <f>IF(B87="","",IF(B87="Error","-",VLOOKUP(B87,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D87" s="4"/>
+      <c r="E87" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3049,17 +3147,17 @@
         <f t="shared" si="2"/>
         <v>86</v>
       </c>
-      <c r="B88" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C88" s="8" t="str">
-        <f>IF(ISBLANK(B88),"",VLOOKUP(B88,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D88" s="6"/>
-      <c r="E88" s="7" t="s">
-        <v>84</v>
+      <c r="B88" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C88" s="6" t="str">
+        <f>IF(B88="","",IF(B88="Error","-",VLOOKUP(B88,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D88" s="4"/>
+      <c r="E88" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3067,17 +3165,17 @@
         <f t="shared" si="2"/>
         <v>87</v>
       </c>
-      <c r="B89" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C89" s="8" t="str">
-        <f>IF(ISBLANK(B89),"",VLOOKUP(B89,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D89" s="6"/>
-      <c r="E89" s="7" t="s">
-        <v>84</v>
+      <c r="B89" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C89" s="6" t="str">
+        <f>IF(B89="","",IF(B89="Error","-",VLOOKUP(B89,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D89" s="4"/>
+      <c r="E89" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3085,17 +3183,17 @@
         <f t="shared" si="2"/>
         <v>88</v>
       </c>
-      <c r="B90" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C90" s="8" t="str">
-        <f>IF(ISBLANK(B90),"",VLOOKUP(B90,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D90" s="6"/>
-      <c r="E90" s="7" t="s">
-        <v>84</v>
+      <c r="B90" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C90" s="6" t="str">
+        <f>IF(B90="","",IF(B90="Error","-",VLOOKUP(B90,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D90" s="4"/>
+      <c r="E90" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3103,17 +3201,17 @@
         <f t="shared" si="2"/>
         <v>89</v>
       </c>
-      <c r="B91" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C91" s="8" t="str">
-        <f>IF(ISBLANK(B91),"",VLOOKUP(B91,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D91" s="6"/>
-      <c r="E91" s="7" t="s">
-        <v>84</v>
+      <c r="B91" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C91" s="6" t="str">
+        <f>IF(B91="","",IF(B91="Error","-",VLOOKUP(B91,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D91" s="4"/>
+      <c r="E91" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3121,17 +3219,17 @@
         <f t="shared" si="2"/>
         <v>90</v>
       </c>
-      <c r="B92" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C92" s="8" t="str">
-        <f>IF(ISBLANK(B92),"",VLOOKUP(B92,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D92" s="6"/>
-      <c r="E92" s="7" t="s">
-        <v>84</v>
+      <c r="B92" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C92" s="6" t="str">
+        <f>IF(B92="","",IF(B92="Error","-",VLOOKUP(B92,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D92" s="4"/>
+      <c r="E92" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3139,17 +3237,17 @@
         <f t="shared" si="2"/>
         <v>91</v>
       </c>
-      <c r="B93" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C93" s="8" t="str">
-        <f>IF(ISBLANK(B93),"",VLOOKUP(B93,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D93" s="6"/>
-      <c r="E93" s="7" t="s">
-        <v>84</v>
+      <c r="B93" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C93" s="6" t="str">
+        <f>IF(B93="","",IF(B93="Error","-",VLOOKUP(B93,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D93" s="4"/>
+      <c r="E93" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3157,17 +3255,17 @@
         <f t="shared" si="2"/>
         <v>92</v>
       </c>
-      <c r="B94" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C94" s="8" t="str">
-        <f>IF(ISBLANK(B94),"",VLOOKUP(B94,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D94" s="6"/>
-      <c r="E94" s="7" t="s">
-        <v>84</v>
+      <c r="B94" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C94" s="6" t="str">
+        <f>IF(B94="","",IF(B94="Error","-",VLOOKUP(B94,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D94" s="4"/>
+      <c r="E94" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3175,17 +3273,17 @@
         <f t="shared" si="2"/>
         <v>93</v>
       </c>
-      <c r="B95" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C95" s="8" t="str">
-        <f>IF(ISBLANK(B95),"",VLOOKUP(B95,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D95" s="6"/>
-      <c r="E95" s="7" t="s">
-        <v>84</v>
+      <c r="B95" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C95" s="6" t="str">
+        <f>IF(B95="","",IF(B95="Error","-",VLOOKUP(B95,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D95" s="4"/>
+      <c r="E95" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3193,17 +3291,17 @@
         <f t="shared" si="2"/>
         <v>94</v>
       </c>
-      <c r="B96" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C96" s="8" t="str">
-        <f>IF(ISBLANK(B96),"",VLOOKUP(B96,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D96" s="6"/>
-      <c r="E96" s="7" t="s">
-        <v>84</v>
+      <c r="B96" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C96" s="6" t="str">
+        <f>IF(B96="","",IF(B96="Error","-",VLOOKUP(B96,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D96" s="4"/>
+      <c r="E96" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3211,17 +3309,17 @@
         <f t="shared" si="2"/>
         <v>95</v>
       </c>
-      <c r="B97" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C97" s="8" t="str">
-        <f>IF(ISBLANK(B97),"",VLOOKUP(B97,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D97" s="6"/>
-      <c r="E97" s="7" t="s">
-        <v>84</v>
+      <c r="B97" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C97" s="6" t="str">
+        <f>IF(B97="","",IF(B97="Error","-",VLOOKUP(B97,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D97" s="4"/>
+      <c r="E97" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3229,17 +3327,17 @@
         <f t="shared" si="2"/>
         <v>96</v>
       </c>
-      <c r="B98" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C98" s="8" t="str">
-        <f>IF(ISBLANK(B98),"",VLOOKUP(B98,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D98" s="6"/>
-      <c r="E98" s="7" t="s">
-        <v>84</v>
+      <c r="B98" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C98" s="6" t="str">
+        <f>IF(B98="","",IF(B98="Error","-",VLOOKUP(B98,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D98" s="4"/>
+      <c r="E98" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3247,17 +3345,17 @@
         <f t="shared" si="2"/>
         <v>97</v>
       </c>
-      <c r="B99" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C99" s="8" t="str">
-        <f>IF(ISBLANK(B99),"",VLOOKUP(B99,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D99" s="6"/>
-      <c r="E99" s="7" t="s">
-        <v>84</v>
+      <c r="B99" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C99" s="6" t="str">
+        <f>IF(B99="","",IF(B99="Error","-",VLOOKUP(B99,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D99" s="4"/>
+      <c r="E99" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3265,17 +3363,17 @@
         <f t="shared" si="2"/>
         <v>98</v>
       </c>
-      <c r="B100" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C100" s="8" t="str">
-        <f>IF(ISBLANK(B100),"",VLOOKUP(B100,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D100" s="6"/>
-      <c r="E100" s="7" t="s">
-        <v>84</v>
+      <c r="B100" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C100" s="6" t="str">
+        <f>IF(B100="","",IF(B100="Error","-",VLOOKUP(B100,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D100" s="4"/>
+      <c r="E100" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3283,17 +3381,17 @@
         <f t="shared" si="2"/>
         <v>99</v>
       </c>
-      <c r="B101" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C101" s="8" t="str">
-        <f>IF(ISBLANK(B101),"",VLOOKUP(B101,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D101" s="6"/>
-      <c r="E101" s="7" t="s">
-        <v>84</v>
+      <c r="B101" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C101" s="6" t="str">
+        <f>IF(B101="","",IF(B101="Error","-",VLOOKUP(B101,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D101" s="4"/>
+      <c r="E101" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3301,17 +3399,17 @@
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
-      <c r="B102" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C102" s="8" t="str">
-        <f>IF(ISBLANK(B102),"",VLOOKUP(B102,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D102" s="6"/>
-      <c r="E102" s="7" t="s">
-        <v>84</v>
+      <c r="B102" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C102" s="6" t="str">
+        <f>IF(B102="","",IF(B102="Error","-",VLOOKUP(B102,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D102" s="4"/>
+      <c r="E102" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3319,17 +3417,17 @@
         <f t="shared" si="2"/>
         <v>101</v>
       </c>
-      <c r="B103" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C103" s="8" t="str">
-        <f>IF(ISBLANK(B103),"",VLOOKUP(B103,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D103" s="6"/>
-      <c r="E103" s="7" t="s">
-        <v>84</v>
+      <c r="B103" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C103" s="6" t="str">
+        <f>IF(B103="","",IF(B103="Error","-",VLOOKUP(B103,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D103" s="4"/>
+      <c r="E103" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3337,17 +3435,17 @@
         <f t="shared" si="2"/>
         <v>102</v>
       </c>
-      <c r="B104" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C104" s="8" t="str">
-        <f>IF(ISBLANK(B104),"",VLOOKUP(B104,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D104" s="6"/>
-      <c r="E104" s="7" t="s">
-        <v>84</v>
+      <c r="B104" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C104" s="6" t="str">
+        <f>IF(B104="","",IF(B104="Error","-",VLOOKUP(B104,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D104" s="4"/>
+      <c r="E104" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3355,17 +3453,17 @@
         <f t="shared" si="2"/>
         <v>103</v>
       </c>
-      <c r="B105" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C105" s="8" t="str">
-        <f>IF(ISBLANK(B105),"",VLOOKUP(B105,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D105" s="6"/>
-      <c r="E105" s="7" t="s">
-        <v>84</v>
+      <c r="B105" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C105" s="6" t="str">
+        <f>IF(B105="","",IF(B105="Error","-",VLOOKUP(B105,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D105" s="4"/>
+      <c r="E105" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3373,17 +3471,17 @@
         <f t="shared" si="2"/>
         <v>104</v>
       </c>
-      <c r="B106" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C106" s="8" t="str">
-        <f>IF(ISBLANK(B106),"",VLOOKUP(B106,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D106" s="6"/>
-      <c r="E106" s="7" t="s">
-        <v>84</v>
+      <c r="B106" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C106" s="6" t="str">
+        <f>IF(B106="","",IF(B106="Error","-",VLOOKUP(B106,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D106" s="4"/>
+      <c r="E106" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3391,17 +3489,17 @@
         <f t="shared" si="2"/>
         <v>105</v>
       </c>
-      <c r="B107" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C107" s="8" t="str">
-        <f>IF(ISBLANK(B107),"",VLOOKUP(B107,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D107" s="6"/>
-      <c r="E107" s="7" t="s">
-        <v>84</v>
+      <c r="B107" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C107" s="6" t="str">
+        <f>IF(B107="","",IF(B107="Error","-",VLOOKUP(B107,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D107" s="4"/>
+      <c r="E107" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3409,17 +3507,17 @@
         <f t="shared" si="2"/>
         <v>106</v>
       </c>
-      <c r="B108" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C108" s="8" t="str">
-        <f>IF(ISBLANK(B108),"",VLOOKUP(B108,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D108" s="6"/>
-      <c r="E108" s="7" t="s">
-        <v>84</v>
+      <c r="B108" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C108" s="6" t="str">
+        <f>IF(B108="","",IF(B108="Error","-",VLOOKUP(B108,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D108" s="4"/>
+      <c r="E108" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3427,17 +3525,17 @@
         <f t="shared" si="2"/>
         <v>107</v>
       </c>
-      <c r="B109" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C109" s="8" t="str">
-        <f>IF(ISBLANK(B109),"",VLOOKUP(B109,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D109" s="6"/>
-      <c r="E109" s="7" t="s">
-        <v>84</v>
+      <c r="B109" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C109" s="6" t="str">
+        <f>IF(B109="","",IF(B109="Error","-",VLOOKUP(B109,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D109" s="4"/>
+      <c r="E109" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3445,17 +3543,17 @@
         <f t="shared" si="2"/>
         <v>108</v>
       </c>
-      <c r="B110" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C110" s="8" t="str">
-        <f>IF(ISBLANK(B110),"",VLOOKUP(B110,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D110" s="6"/>
-      <c r="E110" s="7" t="s">
-        <v>84</v>
+      <c r="B110" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C110" s="6" t="str">
+        <f>IF(B110="","",IF(B110="Error","-",VLOOKUP(B110,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D110" s="4"/>
+      <c r="E110" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3463,17 +3561,17 @@
         <f t="shared" si="2"/>
         <v>109</v>
       </c>
-      <c r="B111" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C111" s="8" t="str">
-        <f>IF(ISBLANK(B111),"",VLOOKUP(B111,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D111" s="6"/>
-      <c r="E111" s="7" t="s">
-        <v>84</v>
+      <c r="B111" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C111" s="6" t="str">
+        <f>IF(B111="","",IF(B111="Error","-",VLOOKUP(B111,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D111" s="4"/>
+      <c r="E111" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3481,17 +3579,17 @@
         <f t="shared" si="2"/>
         <v>110</v>
       </c>
-      <c r="B112" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C112" s="8" t="str">
-        <f>IF(ISBLANK(B112),"",VLOOKUP(B112,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D112" s="6"/>
-      <c r="E112" s="7" t="s">
-        <v>84</v>
+      <c r="B112" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C112" s="6" t="str">
+        <f>IF(B112="","",IF(B112="Error","-",VLOOKUP(B112,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D112" s="4"/>
+      <c r="E112" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3499,17 +3597,17 @@
         <f t="shared" si="2"/>
         <v>111</v>
       </c>
-      <c r="B113" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C113" s="8" t="str">
-        <f>IF(ISBLANK(B113),"",VLOOKUP(B113,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D113" s="6"/>
-      <c r="E113" s="7" t="s">
-        <v>84</v>
+      <c r="B113" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C113" s="6" t="str">
+        <f>IF(B113="","",IF(B113="Error","-",VLOOKUP(B113,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D113" s="4"/>
+      <c r="E113" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3517,17 +3615,17 @@
         <f t="shared" si="2"/>
         <v>112</v>
       </c>
-      <c r="B114" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C114" s="8" t="str">
-        <f>IF(ISBLANK(B114),"",VLOOKUP(B114,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D114" s="6"/>
-      <c r="E114" s="7" t="s">
-        <v>84</v>
+      <c r="B114" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C114" s="6" t="str">
+        <f>IF(B114="","",IF(B114="Error","-",VLOOKUP(B114,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D114" s="4"/>
+      <c r="E114" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3535,17 +3633,17 @@
         <f t="shared" si="2"/>
         <v>113</v>
       </c>
-      <c r="B115" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C115" s="8" t="str">
-        <f>IF(ISBLANK(B115),"",VLOOKUP(B115,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D115" s="6"/>
-      <c r="E115" s="7" t="s">
-        <v>84</v>
+      <c r="B115" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C115" s="6" t="str">
+        <f>IF(B115="","",IF(B115="Error","-",VLOOKUP(B115,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D115" s="4"/>
+      <c r="E115" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3553,17 +3651,17 @@
         <f t="shared" si="2"/>
         <v>114</v>
       </c>
-      <c r="B116" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C116" s="8" t="str">
-        <f>IF(ISBLANK(B116),"",VLOOKUP(B116,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D116" s="6"/>
-      <c r="E116" s="7" t="s">
-        <v>84</v>
+      <c r="B116" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C116" s="6" t="str">
+        <f>IF(B116="","",IF(B116="Error","-",VLOOKUP(B116,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D116" s="4"/>
+      <c r="E116" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3571,17 +3669,17 @@
         <f t="shared" si="2"/>
         <v>115</v>
       </c>
-      <c r="B117" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C117" s="8" t="str">
-        <f>IF(ISBLANK(B117),"",VLOOKUP(B117,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D117" s="6"/>
-      <c r="E117" s="7" t="s">
-        <v>84</v>
+      <c r="B117" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C117" s="6" t="str">
+        <f>IF(B117="","",IF(B117="Error","-",VLOOKUP(B117,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D117" s="4"/>
+      <c r="E117" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3589,17 +3687,17 @@
         <f t="shared" si="2"/>
         <v>116</v>
       </c>
-      <c r="B118" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C118" s="8" t="str">
-        <f>IF(ISBLANK(B118),"",VLOOKUP(B118,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D118" s="6"/>
-      <c r="E118" s="7" t="s">
-        <v>84</v>
+      <c r="B118" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C118" s="6" t="str">
+        <f>IF(B118="","",IF(B118="Error","-",VLOOKUP(B118,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D118" s="4"/>
+      <c r="E118" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3607,17 +3705,17 @@
         <f t="shared" si="2"/>
         <v>117</v>
       </c>
-      <c r="B119" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C119" s="8" t="str">
-        <f>IF(ISBLANK(B119),"",VLOOKUP(B119,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D119" s="6"/>
-      <c r="E119" s="7" t="s">
-        <v>84</v>
+      <c r="B119" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C119" s="6" t="str">
+        <f>IF(B119="","",IF(B119="Error","-",VLOOKUP(B119,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D119" s="4"/>
+      <c r="E119" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3625,17 +3723,17 @@
         <f t="shared" si="2"/>
         <v>118</v>
       </c>
-      <c r="B120" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C120" s="8" t="str">
-        <f>IF(ISBLANK(B120),"",VLOOKUP(B120,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D120" s="6"/>
-      <c r="E120" s="7" t="s">
-        <v>84</v>
+      <c r="B120" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C120" s="6" t="str">
+        <f>IF(B120="","",IF(B120="Error","-",VLOOKUP(B120,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D120" s="4"/>
+      <c r="E120" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3643,17 +3741,17 @@
         <f t="shared" si="2"/>
         <v>119</v>
       </c>
-      <c r="B121" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C121" s="8" t="str">
-        <f>IF(ISBLANK(B121),"",VLOOKUP(B121,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D121" s="6"/>
-      <c r="E121" s="7" t="s">
-        <v>84</v>
+      <c r="B121" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C121" s="6" t="str">
+        <f>IF(B121="","",IF(B121="Error","-",VLOOKUP(B121,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D121" s="4"/>
+      <c r="E121" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3661,17 +3759,17 @@
         <f t="shared" si="2"/>
         <v>120</v>
       </c>
-      <c r="B122" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C122" s="8" t="str">
-        <f>IF(ISBLANK(B122),"",VLOOKUP(B122,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D122" s="6"/>
-      <c r="E122" s="7" t="s">
-        <v>84</v>
+      <c r="B122" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C122" s="6" t="str">
+        <f>IF(B122="","",IF(B122="Error","-",VLOOKUP(B122,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D122" s="4"/>
+      <c r="E122" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3679,17 +3777,17 @@
         <f t="shared" si="2"/>
         <v>121</v>
       </c>
-      <c r="B123" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C123" s="8" t="str">
-        <f>IF(ISBLANK(B123),"",VLOOKUP(B123,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D123" s="6"/>
-      <c r="E123" s="7" t="s">
-        <v>84</v>
+      <c r="B123" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C123" s="6" t="str">
+        <f>IF(B123="","",IF(B123="Error","-",VLOOKUP(B123,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D123" s="4"/>
+      <c r="E123" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3697,17 +3795,17 @@
         <f t="shared" si="2"/>
         <v>122</v>
       </c>
-      <c r="B124" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C124" s="8" t="str">
-        <f>IF(ISBLANK(B124),"",VLOOKUP(B124,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D124" s="6"/>
-      <c r="E124" s="7" t="s">
-        <v>84</v>
+      <c r="B124" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C124" s="6" t="str">
+        <f>IF(B124="","",IF(B124="Error","-",VLOOKUP(B124,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D124" s="4"/>
+      <c r="E124" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3715,17 +3813,17 @@
         <f t="shared" si="2"/>
         <v>123</v>
       </c>
-      <c r="B125" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C125" s="8" t="str">
-        <f>IF(ISBLANK(B125),"",VLOOKUP(B125,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D125" s="6"/>
-      <c r="E125" s="7" t="s">
-        <v>84</v>
+      <c r="B125" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C125" s="6" t="str">
+        <f>IF(B125="","",IF(B125="Error","-",VLOOKUP(B125,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D125" s="4"/>
+      <c r="E125" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3733,17 +3831,17 @@
         <f t="shared" si="2"/>
         <v>124</v>
       </c>
-      <c r="B126" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C126" s="8" t="str">
-        <f>IF(ISBLANK(B126),"",VLOOKUP(B126,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D126" s="6"/>
-      <c r="E126" s="7" t="s">
-        <v>84</v>
+      <c r="B126" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C126" s="6" t="str">
+        <f>IF(B126="","",IF(B126="Error","-",VLOOKUP(B126,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D126" s="4"/>
+      <c r="E126" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3751,17 +3849,17 @@
         <f t="shared" si="2"/>
         <v>125</v>
       </c>
-      <c r="B127" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C127" s="8" t="str">
-        <f>IF(ISBLANK(B127),"",VLOOKUP(B127,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D127" s="6"/>
-      <c r="E127" s="7" t="s">
-        <v>84</v>
+      <c r="B127" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C127" s="6" t="str">
+        <f>IF(B127="","",IF(B127="Error","-",VLOOKUP(B127,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D127" s="4"/>
+      <c r="E127" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3769,17 +3867,17 @@
         <f t="shared" si="2"/>
         <v>126</v>
       </c>
-      <c r="B128" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C128" s="8" t="str">
-        <f>IF(ISBLANK(B128),"",VLOOKUP(B128,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D128" s="6"/>
-      <c r="E128" s="7" t="s">
-        <v>84</v>
+      <c r="B128" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C128" s="6" t="str">
+        <f>IF(B128="","",IF(B128="Error","-",VLOOKUP(B128,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D128" s="4"/>
+      <c r="E128" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3787,17 +3885,17 @@
         <f t="shared" si="2"/>
         <v>127</v>
       </c>
-      <c r="B129" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C129" s="8" t="str">
-        <f>IF(ISBLANK(B129),"",VLOOKUP(B129,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D129" s="6"/>
-      <c r="E129" s="7" t="s">
-        <v>84</v>
+      <c r="B129" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C129" s="6" t="str">
+        <f>IF(B129="","",IF(B129="Error","-",VLOOKUP(B129,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D129" s="4"/>
+      <c r="E129" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3805,17 +3903,17 @@
         <f t="shared" si="2"/>
         <v>128</v>
       </c>
-      <c r="B130" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C130" s="8" t="str">
-        <f>IF(ISBLANK(B130),"",VLOOKUP(B130,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D130" s="6"/>
-      <c r="E130" s="7" t="s">
-        <v>84</v>
+      <c r="B130" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C130" s="6" t="str">
+        <f>IF(B130="","",IF(B130="Error","-",VLOOKUP(B130,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D130" s="4"/>
+      <c r="E130" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3823,17 +3921,17 @@
         <f t="shared" si="2"/>
         <v>129</v>
       </c>
-      <c r="B131" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C131" s="8" t="str">
-        <f>IF(ISBLANK(B131),"",VLOOKUP(B131,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D131" s="6"/>
-      <c r="E131" s="7" t="s">
-        <v>84</v>
+      <c r="B131" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C131" s="6" t="str">
+        <f>IF(B131="","",IF(B131="Error","-",VLOOKUP(B131,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D131" s="4"/>
+      <c r="E131" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3841,17 +3939,17 @@
         <f t="shared" si="2"/>
         <v>130</v>
       </c>
-      <c r="B132" s="6">
-        <f t="shared" si="3"/>
-        <v>8</v>
-      </c>
-      <c r="C132" s="8" t="str">
-        <f>IF(ISBLANK(B132),"",VLOOKUP(B132,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D132" s="6"/>
-      <c r="E132" s="7" t="s">
-        <v>84</v>
+      <c r="B132" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="C132" s="6" t="str">
+        <f>IF(B132="","",IF(B132="Error","-",VLOOKUP(B132,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D132" s="4"/>
+      <c r="E132" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3859,17 +3957,17 @@
         <f t="shared" ref="A133:A152" si="4">A132+1</f>
         <v>131</v>
       </c>
-      <c r="B133" s="6">
-        <f t="shared" ref="B133:B152" si="5">IF(D132="Check",B132+1,B132)</f>
-        <v>8</v>
-      </c>
-      <c r="C133" s="8" t="str">
-        <f>IF(ISBLANK(B133),"",VLOOKUP(B133,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D133" s="6"/>
-      <c r="E133" s="7" t="s">
-        <v>84</v>
+      <c r="B133" s="4" t="str">
+        <f t="shared" ref="B133:B152" si="5">IF(ISBLANK(D132),"",IF(D132="Check",B132+1,IF(D132="Fail",B132,"Error")))</f>
+        <v/>
+      </c>
+      <c r="C133" s="6" t="str">
+        <f>IF(B133="","",IF(B133="Error","-",VLOOKUP(B133,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D133" s="4"/>
+      <c r="E133" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3877,17 +3975,17 @@
         <f t="shared" si="4"/>
         <v>132</v>
       </c>
-      <c r="B134" s="6">
+      <c r="B134" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="C134" s="8" t="str">
-        <f>IF(ISBLANK(B134),"",VLOOKUP(B134,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D134" s="6"/>
-      <c r="E134" s="7" t="s">
-        <v>84</v>
+        <v/>
+      </c>
+      <c r="C134" s="6" t="str">
+        <f>IF(B134="","",IF(B134="Error","-",VLOOKUP(B134,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D134" s="4"/>
+      <c r="E134" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3895,17 +3993,17 @@
         <f t="shared" si="4"/>
         <v>133</v>
       </c>
-      <c r="B135" s="6">
+      <c r="B135" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="C135" s="8" t="str">
-        <f>IF(ISBLANK(B135),"",VLOOKUP(B135,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D135" s="6"/>
-      <c r="E135" s="7" t="s">
-        <v>84</v>
+        <v/>
+      </c>
+      <c r="C135" s="6" t="str">
+        <f>IF(B135="","",IF(B135="Error","-",VLOOKUP(B135,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D135" s="4"/>
+      <c r="E135" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3913,17 +4011,17 @@
         <f t="shared" si="4"/>
         <v>134</v>
       </c>
-      <c r="B136" s="6">
+      <c r="B136" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="C136" s="8" t="str">
-        <f>IF(ISBLANK(B136),"",VLOOKUP(B136,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D136" s="6"/>
-      <c r="E136" s="7" t="s">
-        <v>84</v>
+        <v/>
+      </c>
+      <c r="C136" s="6" t="str">
+        <f>IF(B136="","",IF(B136="Error","-",VLOOKUP(B136,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D136" s="4"/>
+      <c r="E136" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3931,17 +4029,17 @@
         <f t="shared" si="4"/>
         <v>135</v>
       </c>
-      <c r="B137" s="6">
+      <c r="B137" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="C137" s="8" t="str">
-        <f>IF(ISBLANK(B137),"",VLOOKUP(B137,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D137" s="6"/>
-      <c r="E137" s="7" t="s">
-        <v>84</v>
+        <v/>
+      </c>
+      <c r="C137" s="6" t="str">
+        <f>IF(B137="","",IF(B137="Error","-",VLOOKUP(B137,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D137" s="4"/>
+      <c r="E137" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3949,17 +4047,17 @@
         <f t="shared" si="4"/>
         <v>136</v>
       </c>
-      <c r="B138" s="6">
+      <c r="B138" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="C138" s="8" t="str">
-        <f>IF(ISBLANK(B138),"",VLOOKUP(B138,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D138" s="6"/>
-      <c r="E138" s="7" t="s">
-        <v>84</v>
+        <v/>
+      </c>
+      <c r="C138" s="6" t="str">
+        <f>IF(B138="","",IF(B138="Error","-",VLOOKUP(B138,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D138" s="4"/>
+      <c r="E138" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="139" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3967,17 +4065,17 @@
         <f t="shared" si="4"/>
         <v>137</v>
       </c>
-      <c r="B139" s="6">
+      <c r="B139" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="C139" s="8" t="str">
-        <f>IF(ISBLANK(B139),"",VLOOKUP(B139,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D139" s="6"/>
-      <c r="E139" s="7" t="s">
-        <v>84</v>
+        <v/>
+      </c>
+      <c r="C139" s="6" t="str">
+        <f>IF(B139="","",IF(B139="Error","-",VLOOKUP(B139,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D139" s="4"/>
+      <c r="E139" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -3985,17 +4083,17 @@
         <f t="shared" si="4"/>
         <v>138</v>
       </c>
-      <c r="B140" s="6">
+      <c r="B140" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="C140" s="8" t="str">
-        <f>IF(ISBLANK(B140),"",VLOOKUP(B140,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D140" s="6"/>
-      <c r="E140" s="7" t="s">
-        <v>84</v>
+        <v/>
+      </c>
+      <c r="C140" s="6" t="str">
+        <f>IF(B140="","",IF(B140="Error","-",VLOOKUP(B140,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D140" s="4"/>
+      <c r="E140" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="141" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -4003,17 +4101,17 @@
         <f t="shared" si="4"/>
         <v>139</v>
       </c>
-      <c r="B141" s="6">
+      <c r="B141" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="C141" s="8" t="str">
-        <f>IF(ISBLANK(B141),"",VLOOKUP(B141,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D141" s="6"/>
-      <c r="E141" s="7" t="s">
-        <v>84</v>
+        <v/>
+      </c>
+      <c r="C141" s="6" t="str">
+        <f>IF(B141="","",IF(B141="Error","-",VLOOKUP(B141,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D141" s="4"/>
+      <c r="E141" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -4021,17 +4119,17 @@
         <f t="shared" si="4"/>
         <v>140</v>
       </c>
-      <c r="B142" s="6">
+      <c r="B142" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="C142" s="8" t="str">
-        <f>IF(ISBLANK(B142),"",VLOOKUP(B142,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D142" s="6"/>
-      <c r="E142" s="7" t="s">
-        <v>84</v>
+        <v/>
+      </c>
+      <c r="C142" s="6" t="str">
+        <f>IF(B142="","",IF(B142="Error","-",VLOOKUP(B142,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D142" s="4"/>
+      <c r="E142" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -4039,17 +4137,17 @@
         <f t="shared" si="4"/>
         <v>141</v>
       </c>
-      <c r="B143" s="6">
+      <c r="B143" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="C143" s="8" t="str">
-        <f>IF(ISBLANK(B143),"",VLOOKUP(B143,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D143" s="6"/>
-      <c r="E143" s="7" t="s">
-        <v>84</v>
+        <v/>
+      </c>
+      <c r="C143" s="6" t="str">
+        <f>IF(B143="","",IF(B143="Error","-",VLOOKUP(B143,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D143" s="4"/>
+      <c r="E143" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -4057,17 +4155,17 @@
         <f t="shared" si="4"/>
         <v>142</v>
       </c>
-      <c r="B144" s="6">
+      <c r="B144" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="C144" s="8" t="str">
-        <f>IF(ISBLANK(B144),"",VLOOKUP(B144,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D144" s="6"/>
-      <c r="E144" s="7" t="s">
-        <v>84</v>
+        <v/>
+      </c>
+      <c r="C144" s="6" t="str">
+        <f>IF(B144="","",IF(B144="Error","-",VLOOKUP(B144,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D144" s="4"/>
+      <c r="E144" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="145" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -4075,17 +4173,17 @@
         <f t="shared" si="4"/>
         <v>143</v>
       </c>
-      <c r="B145" s="6">
+      <c r="B145" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="C145" s="8" t="str">
-        <f>IF(ISBLANK(B145),"",VLOOKUP(B145,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D145" s="6"/>
-      <c r="E145" s="7" t="s">
-        <v>84</v>
+        <v/>
+      </c>
+      <c r="C145" s="6" t="str">
+        <f>IF(B145="","",IF(B145="Error","-",VLOOKUP(B145,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D145" s="4"/>
+      <c r="E145" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="146" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -4093,17 +4191,17 @@
         <f t="shared" si="4"/>
         <v>144</v>
       </c>
-      <c r="B146" s="6">
+      <c r="B146" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="C146" s="8" t="str">
-        <f>IF(ISBLANK(B146),"",VLOOKUP(B146,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D146" s="6"/>
-      <c r="E146" s="7" t="s">
-        <v>84</v>
+        <v/>
+      </c>
+      <c r="C146" s="6" t="str">
+        <f>IF(B146="","",IF(B146="Error","-",VLOOKUP(B146,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D146" s="4"/>
+      <c r="E146" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="147" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -4111,17 +4209,17 @@
         <f t="shared" si="4"/>
         <v>145</v>
       </c>
-      <c r="B147" s="6">
+      <c r="B147" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="C147" s="8" t="str">
-        <f>IF(ISBLANK(B147),"",VLOOKUP(B147,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D147" s="6"/>
-      <c r="E147" s="7" t="s">
-        <v>84</v>
+        <v/>
+      </c>
+      <c r="C147" s="6" t="str">
+        <f>IF(B147="","",IF(B147="Error","-",VLOOKUP(B147,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D147" s="4"/>
+      <c r="E147" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="148" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -4129,17 +4227,17 @@
         <f t="shared" si="4"/>
         <v>146</v>
       </c>
-      <c r="B148" s="6">
+      <c r="B148" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="C148" s="8" t="str">
-        <f>IF(ISBLANK(B148),"",VLOOKUP(B148,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D148" s="6"/>
-      <c r="E148" s="7" t="s">
-        <v>84</v>
+        <v/>
+      </c>
+      <c r="C148" s="6" t="str">
+        <f>IF(B148="","",IF(B148="Error","-",VLOOKUP(B148,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D148" s="4"/>
+      <c r="E148" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="149" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -4147,17 +4245,17 @@
         <f t="shared" si="4"/>
         <v>147</v>
       </c>
-      <c r="B149" s="6">
+      <c r="B149" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="C149" s="8" t="str">
-        <f>IF(ISBLANK(B149),"",VLOOKUP(B149,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D149" s="6"/>
-      <c r="E149" s="7" t="s">
-        <v>84</v>
+        <v/>
+      </c>
+      <c r="C149" s="6" t="str">
+        <f>IF(B149="","",IF(B149="Error","-",VLOOKUP(B149,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D149" s="4"/>
+      <c r="E149" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="150" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -4165,17 +4263,17 @@
         <f t="shared" si="4"/>
         <v>148</v>
       </c>
-      <c r="B150" s="6">
+      <c r="B150" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="C150" s="8" t="str">
-        <f>IF(ISBLANK(B150),"",VLOOKUP(B150,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D150" s="6"/>
-      <c r="E150" s="7" t="s">
-        <v>84</v>
+        <v/>
+      </c>
+      <c r="C150" s="6" t="str">
+        <f>IF(B150="","",IF(B150="Error","-",VLOOKUP(B150,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D150" s="4"/>
+      <c r="E150" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="151" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -4183,17 +4281,17 @@
         <f t="shared" si="4"/>
         <v>149</v>
       </c>
-      <c r="B151" s="6">
+      <c r="B151" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="C151" s="8" t="str">
-        <f>IF(ISBLANK(B151),"",VLOOKUP(B151,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D151" s="6"/>
-      <c r="E151" s="7" t="s">
-        <v>84</v>
+        <v/>
+      </c>
+      <c r="C151" s="6" t="str">
+        <f>IF(B151="","",IF(B151="Error","-",VLOOKUP(B151,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D151" s="4"/>
+      <c r="E151" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="152" spans="1:5" ht="15" x14ac:dyDescent="0.3">
@@ -4201,17 +4299,17 @@
         <f t="shared" si="4"/>
         <v>150</v>
       </c>
-      <c r="B152" s="6">
+      <c r="B152" s="4" t="str">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="C152" s="8" t="str">
-        <f>IF(ISBLANK(B152),"",VLOOKUP(B152,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE))</f>
-        <v>Testing closing the game using a simple timer and stoping the thread</v>
-      </c>
-      <c r="D152" s="6"/>
-      <c r="E152" s="7" t="s">
-        <v>84</v>
+        <v/>
+      </c>
+      <c r="C152" s="6" t="str">
+        <f>IF(B152="","",IF(B152="Error","-",VLOOKUP(B152,'Iteratives Development Steps'!$A$3:$B$200,2,FALSE)))</f>
+        <v/>
+      </c>
+      <c r="D152" s="4"/>
+      <c r="E152" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>